<commit_message>
modified traverse function to add subjects from dss to sodajsonobj
</commit_message>
<xml_diff>
--- a/src/submission.xlsx
+++ b/src/submission.xlsx
@@ -479,7 +479,7 @@
       </c>
       <c r="C2" s="11" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -496,7 +496,7 @@
       </c>
       <c r="C3" s="11" t="inlineStr">
         <is>
-          <t>232</t>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -513,7 +513,7 @@
       </c>
       <c r="C4" s="11" t="inlineStr">
         <is>
-          <t>2022-03-23</t>
+          <t>2022-03-31</t>
         </is>
       </c>
     </row>

</xml_diff>